<commit_message>
Completing Dunns Test Results.
</commit_message>
<xml_diff>
--- a/ANOVA/DunnTestDOI.xlsx
+++ b/ANOVA/DunnTestDOI.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_Package_Cbone_FIRES\Code\Fire_Analysis_2020\ANOVA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\R_Package_Cbone_FIRES\Code\Fire_Analysis_2020\ANOVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5508178-0F98-439F-9C8A-20000D56DD7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11895" yWindow="5520" windowWidth="18000" windowHeight="9360" tabRatio="866" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11895" yWindow="5520" windowWidth="18000" windowHeight="9360" tabRatio="866" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="DunnTest_PM2.5_DOI" sheetId="8" r:id="rId1"/>
@@ -248,7 +247,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1163,7 +1162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2489,7 +2488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3813,11 +3812,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:P13"/>
+    <sheetView topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5144,11 +5143,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:P13"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6470,11 +6469,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:Q13"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7796,11 +7795,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:P13"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9123,11 +9122,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:P13"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>